<commit_message>
added time to go off road prediction
</commit_message>
<xml_diff>
--- a/experiment_log.xlsx
+++ b/experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -796,10 +796,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>002</t>
-        </is>
+      <c r="A17" t="n">
+        <v>2</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -817,6 +815,470 @@
       </c>
       <c r="F17" t="n">
         <v>17.92</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>24.55</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10.36</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" t="n">
+        <v>82.81999999999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>29.01</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7.39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Visual Only</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>66.64</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>7</v>
+      </c>
+      <c r="F28" t="n">
+        <v>26.32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>11</v>
+      </c>
+      <c r="F29" t="n">
+        <v>33.44</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4</v>
+      </c>
+      <c r="F30" t="n">
+        <v>48.81</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4</v>
+      </c>
+      <c r="F31" t="n">
+        <v>26.26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5</v>
+      </c>
+      <c r="F32" t="n">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12</v>
+      </c>
+      <c r="F33" t="n">
+        <v>44.22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>23.18</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" t="n">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>7</v>
+      </c>
+      <c r="F37" t="n">
+        <v>34.27</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6</v>
+      </c>
+      <c r="F38" t="n">
+        <v>41.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added haptic feedback and 1st person camera
</commit_message>
<xml_diff>
--- a/experiment_log.xlsx
+++ b/experiment_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1258,10 +1258,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>002</t>
-        </is>
+      <c r="A38" t="n">
+        <v>2</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1279,6 +1277,1328 @@
       </c>
       <c r="F38" t="n">
         <v>41.92</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F40" t="n">
+        <v>60.56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>17</v>
+      </c>
+      <c r="F41" t="n">
+        <v>38.71</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" t="n">
+        <v>19.69</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>7</v>
+      </c>
+      <c r="F44" t="n">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>17</v>
+      </c>
+      <c r="F46" t="n">
+        <v>45.37</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>7</v>
+      </c>
+      <c r="F49" t="n">
+        <v>18.93</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>16</v>
+      </c>
+      <c r="F50" t="n">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>9</v>
+      </c>
+      <c r="F51" t="n">
+        <v>25.68</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="n">
+        <v>11.93</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3</v>
+      </c>
+      <c r="F54" t="n">
+        <v>14.13</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>8</v>
+      </c>
+      <c r="F55" t="n">
+        <v>34.61</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>16</v>
+      </c>
+      <c r="F57" t="n">
+        <v>65.73999999999999</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="n">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4</v>
+      </c>
+      <c r="F60" t="n">
+        <v>27.43</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4</v>
+      </c>
+      <c r="F61" t="n">
+        <v>26.77</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>5</v>
+      </c>
+      <c r="F62" t="n">
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="n">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="n">
+        <v>23.46</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" t="n">
+        <v>10.86</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12.41</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" t="n">
+        <v>10.11</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>25.91</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>3</v>
+      </c>
+      <c r="F72" t="n">
+        <v>24.38</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3</v>
+      </c>
+      <c r="F74" t="n">
+        <v>37.13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="n">
+        <v>8.630000000000001</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>2</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>3</v>
+      </c>
+      <c r="F76" t="n">
+        <v>83.98999999999999</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" t="n">
+        <v>41.92</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4</v>
+      </c>
+      <c r="F78" t="n">
+        <v>61.45</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>2</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>3</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>4</v>
+      </c>
+      <c r="F79" t="n">
+        <v>30.15</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>2</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>7</v>
+      </c>
+      <c r="F81" t="n">
+        <v>35.52</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2</v>
+      </c>
+      <c r="F82" t="n">
+        <v>35.72</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3</v>
+      </c>
+      <c r="F83" t="n">
+        <v>10.21</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>8</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" t="n">
+        <v>37.01</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>2</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>No Feedback</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>5</v>
+      </c>
+      <c r="F85" t="n">
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>10</v>
+      </c>
+      <c r="F86" t="n">
+        <v>40.08</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>9</v>
+      </c>
+      <c r="F88" t="n">
+        <v>20.27</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>2</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>2</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>19</v>
+      </c>
+      <c r="F90" t="n">
+        <v>35.68</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>12</v>
+      </c>
+      <c r="F91" t="n">
+        <v>17.63</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>9</v>
+      </c>
+      <c r="F92" t="n">
+        <v>50.36</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>18</v>
+      </c>
+      <c r="F93" t="n">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>2</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>9</v>
+      </c>
+      <c r="F94" t="n">
+        <v>54.17</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>2</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>5</v>
+      </c>
+      <c r="F95" t="n">
+        <v>10.43</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>2</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>11</v>
+      </c>
+      <c r="F96" t="n">
+        <v>71.34</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>10</v>
+      </c>
+      <c r="F97" t="n">
+        <v>29.88</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Audio Only</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>6.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added GUI for running experiment
</commit_message>
<xml_diff>
--- a/experiment_log.xlsx
+++ b/experiment_log.xlsx
@@ -1,37 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szypy\Desktop\AEM\aem_drive\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6A9CB8-59DA-4AD8-B703-5F9F70ABD67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2760" yWindow="2745" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>experimenter_id</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>n_math_correct</t>
+  </si>
+  <si>
+    <t>n_math_incorrect</t>
+  </si>
+  <si>
+    <t>n_math_timeout</t>
+  </si>
+  <si>
+    <t>time_offroad</t>
+  </si>
+  <si>
+    <t>completion_time</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +78,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,106 +402,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>experimenter_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>n_math_correct</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n_math_incorrect</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>n_math_timeout</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>time_offroad</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>completion_time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>visual</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4.87</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>visual</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="G3" t="n">
-        <v>27.44</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added results from 17 participants
</commit_message>
<xml_diff>
--- a/experiment_log.xlsx
+++ b/experiment_log.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szypy\Desktop\AEM\aem_drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6A9CB8-59DA-4AD8-B703-5F9F70ABD67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA2398B-4B08-4C3C-B24C-AF47E3903AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2745" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
   <si>
     <t>experimenter_id</t>
   </si>
@@ -41,6 +54,24 @@
   </si>
   <si>
     <t>completion_time</t>
+  </si>
+  <si>
+    <t>Unnamed: 7</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>haptic</t>
+  </si>
+  <si>
+    <t>visual</t>
+  </si>
+  <si>
+    <t>no license</t>
   </si>
 </sst>
 </file>
@@ -403,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,6 +463,1597 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2.8458000000000001</v>
+      </c>
+      <c r="G2">
+        <v>44.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1.9184000000000001</v>
+      </c>
+      <c r="G3">
+        <v>53.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1.5294000000000001</v>
+      </c>
+      <c r="G4">
+        <v>49.07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2.4152999999999998</v>
+      </c>
+      <c r="G5">
+        <v>47.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="G6">
+        <v>35.83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.39710000000000001</v>
+      </c>
+      <c r="G7">
+        <v>35.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.3296</v>
+      </c>
+      <c r="G8">
+        <v>35.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.55869999999999997</v>
+      </c>
+      <c r="G9">
+        <v>35.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1.7379</v>
+      </c>
+      <c r="G10">
+        <v>41.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>3.6244999999999998</v>
+      </c>
+      <c r="G11">
+        <v>39.159999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2.7357</v>
+      </c>
+      <c r="G12">
+        <v>41.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>2.1387</v>
+      </c>
+      <c r="G13">
+        <v>38.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>2.4685999999999999</v>
+      </c>
+      <c r="G14">
+        <v>40.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2.5194000000000001</v>
+      </c>
+      <c r="G15">
+        <v>38.53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2.2147000000000001</v>
+      </c>
+      <c r="G16">
+        <v>38.799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1.9467000000000001</v>
+      </c>
+      <c r="G17">
+        <v>39.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>6.2145000000000001</v>
+      </c>
+      <c r="G18">
+        <v>45.24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>3.1394000000000002</v>
+      </c>
+      <c r="G19">
+        <v>37.35</v>
+      </c>
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>6.8876999999999997</v>
+      </c>
+      <c r="G20">
+        <v>45.93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>3.5968</v>
+      </c>
+      <c r="G21">
+        <v>36.81</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>3.133</v>
+      </c>
+      <c r="G22">
+        <v>37.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>4.6314000000000002</v>
+      </c>
+      <c r="G23">
+        <v>43.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>2.5739999999999998</v>
+      </c>
+      <c r="G24">
+        <v>38.520000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1.2023999999999999</v>
+      </c>
+      <c r="G25">
+        <v>37.630000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>3.9036</v>
+      </c>
+      <c r="G26">
+        <v>49.18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1.3720000000000001</v>
+      </c>
+      <c r="G27">
+        <v>45.29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>4.3262</v>
+      </c>
+      <c r="G28">
+        <v>46.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>2.2454000000000001</v>
+      </c>
+      <c r="G29">
+        <v>40.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0.95279999999999998</v>
+      </c>
+      <c r="G30">
+        <v>36.42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>3.7012999999999998</v>
+      </c>
+      <c r="G31">
+        <v>41.81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1.1465000000000001</v>
+      </c>
+      <c r="G32">
+        <v>36.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0.96850000000000003</v>
+      </c>
+      <c r="G33">
+        <v>36.450000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>3.5891999999999999</v>
+      </c>
+      <c r="G34">
+        <v>40.24</v>
+      </c>
+      <c r="H34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>3.2776999999999998</v>
+      </c>
+      <c r="G35">
+        <v>45.38</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>5.6391999999999998</v>
+      </c>
+      <c r="G36">
+        <v>47.66</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>2.3893</v>
+      </c>
+      <c r="G37">
+        <v>38.08</v>
+      </c>
+      <c r="H37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>21</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1.8346</v>
+      </c>
+      <c r="G38">
+        <v>52.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1.8619000000000001</v>
+      </c>
+      <c r="G39">
+        <v>54.36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>24</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="G40">
+        <v>48.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0.90280000000000005</v>
+      </c>
+      <c r="G41">
+        <v>49.92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1.0486</v>
+      </c>
+      <c r="G42">
+        <v>42.51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0.90969999999999995</v>
+      </c>
+      <c r="G43">
+        <v>42.54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>3.3064</v>
+      </c>
+      <c r="G44">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0.71379999999999999</v>
+      </c>
+      <c r="G45">
+        <v>44.51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1.1749000000000001</v>
+      </c>
+      <c r="G46">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0.69179999999999997</v>
+      </c>
+      <c r="G47">
+        <v>36.96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0.68279999999999996</v>
+      </c>
+      <c r="G48">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0.3054</v>
+      </c>
+      <c r="G49">
+        <v>36.659999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>14</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>2.3525</v>
+      </c>
+      <c r="G50">
+        <v>52.47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3.72</v>
+      </c>
+      <c r="G51">
+        <v>46.53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>2.9114</v>
+      </c>
+      <c r="G52">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>3.1173999999999999</v>
+      </c>
+      <c r="G53">
+        <v>43.17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>3.2172999999999998</v>
+      </c>
+      <c r="G54">
+        <v>58.17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>3.0762</v>
+      </c>
+      <c r="G55">
+        <v>51.23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1.7022999999999999</v>
+      </c>
+      <c r="G56">
+        <v>54.14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>1.7964</v>
+      </c>
+      <c r="G57">
+        <v>50.63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>5.3556999999999997</v>
+      </c>
+      <c r="G58">
+        <v>46.61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>9</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>1.5251999999999999</v>
+      </c>
+      <c r="G59">
+        <v>43.43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>15</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>9</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>3.8123999999999998</v>
+      </c>
+      <c r="G60">
+        <v>51.38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>15</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>1.6558999999999999</v>
+      </c>
+      <c r="G61">
+        <v>46.72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>4.2088999999999999</v>
+      </c>
+      <c r="G62">
+        <v>42.38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>0.7681</v>
+      </c>
+      <c r="G63">
+        <v>42.39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>1.8067</v>
+      </c>
+      <c r="G64">
+        <v>37.86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>1.7213000000000001</v>
+      </c>
+      <c r="G65">
+        <v>38.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>17</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <v>21</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>6.4047000000000001</v>
+      </c>
+      <c r="G66">
+        <v>76.63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+      <c r="D67">
+        <v>8</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>1.2099</v>
+      </c>
+      <c r="G67">
+        <v>62.74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>17</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>13</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>3.4129</v>
+      </c>
+      <c r="G68">
+        <v>52.89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>17</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>12</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>5.5239000000000003</v>
+      </c>
+      <c r="G69">
+        <v>46.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>